<commit_message>
Change logic in SMS Bulking, parameter accepting when uploading excel data is (Phone Number and Account Number)
</commit_message>
<xml_diff>
--- a/downloads/sms_deac_bulk.xlsx
+++ b/downloads/sms_deac_bulk.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PortalPilot\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D06C9A-1597-4C11-9D09-45EECB5492E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9068157-01C4-45FD-98B9-ABF770DDCC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{445FB331-9226-4A81-BC99-47DF256F7C61}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>phone number</t>
   </si>
@@ -33,21 +33,12 @@
     <t>account number</t>
   </si>
   <si>
-    <t>email address</t>
-  </si>
-  <si>
     <t>082392042422</t>
   </si>
   <si>
-    <t>princealvinyusuf@gmail.com</t>
-  </si>
-  <si>
     <t>081234982349</t>
   </si>
   <si>
-    <t>abdul@gmail.com</t>
-  </si>
-  <si>
     <t>166010208705285</t>
   </si>
   <si>
@@ -55,9 +46,6 @@
   </si>
   <si>
     <t>1660XXXXXXXX758</t>
-  </si>
-  <si>
-    <t>tag</t>
   </si>
 </sst>
 </file>
@@ -93,12 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,74 +398,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36278383-A2AA-482F-B040-2A335996125D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>